<commit_message>
fix #683: fixed bugs in tutorial notebooks: -added xlrd and openpyxl as dependencies in environment.yml -added cell to display the currently used version of LArray in all tutorial notebooks -fixed the last cell of the notebook tutorial_presenting_larray_objects -replaced calls to array_equals (deprecated in version 0.29) by calls to element_equals in the notebook tutorial_sessions -transformed code cells containing calls to open_excel() to markdown cells -removed calls to open_excel in the last section (i.e. Dumping Sessions) -replaced axis geo by country in tutorial_IO notebook + doctests of read_csv/excel/hdf
</commit_message>
<xml_diff>
--- a/larray/tests/data/births_and_deaths.xlsx
+++ b/larray/tests/data/births_and_deaths.xlsx
@@ -8,18 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ald\Projects\larray\larray\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD70DFDB-0A99-4A85-81D6-836CF1A8CF56}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFAD1122-7EAE-4F3B-95A9-84EB310370EF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11505" activeTab="1" xr2:uid="{B2C3A429-FC47-4D99-A7F6-D8A8C3F4E1FC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11565" activeTab="1" xr2:uid="{9387C5C7-2FAA-42A1-8019-F30B6E5C2081}"/>
   </bookViews>
   <sheets>
-    <sheet name="births" sheetId="2" r:id="rId1"/>
-    <sheet name="deaths" sheetId="3" r:id="rId2"/>
+    <sheet name="births" sheetId="1" r:id="rId1"/>
+    <sheet name="deaths" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -28,7 +33,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
   <si>
-    <t>geo</t>
+    <t>country</t>
   </si>
   <si>
     <t>gender\time</t>
@@ -397,7 +402,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6396E776-1711-4568-A719-12B966118E04}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFB45555-6327-4AD6-B30D-E219C14A99C0}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -529,12 +534,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{797F5477-7C67-4C71-B2D1-2FCA9830F8A7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397585D3-391C-4528-ABD2-321B6C570E76}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
updated tutorial: - added generate_data.py module to generate the example and test data - renamed 'population_session' dataset as 'demography_eurostat' - included values for years 2016 and 2017 for all arrays of 'demography_eurostat' - fix #785 - added the 'Pythonic VS String Syntax' section - updated all existing sections to include changes up to the 0.31 release version
</commit_message>
<xml_diff>
--- a/larray/tests/data/births_and_deaths.xlsx
+++ b/larray/tests/data/births_and_deaths.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ald\Projects\larray\larray\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFAD1122-7EAE-4F3B-95A9-84EB310370EF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CF88169-372B-498A-87CF-E26639E34B81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11565" activeTab="1" xr2:uid="{9387C5C7-2FAA-42A1-8019-F30B6E5C2081}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{5CD7B718-4268-44E7-9AF7-549DB247CE6F}"/>
   </bookViews>
   <sheets>
     <sheet name="births" sheetId="1" r:id="rId1"/>
     <sheet name="deaths" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -402,7 +403,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFB45555-6327-4AD6-B30D-E219C14A99C0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165C2292-4DE4-4BAA-8B67-A256A9BEB0AF}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -534,7 +535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397585D3-391C-4528-ABD2-321B6C570E76}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{510F0CAE-B993-4579-A875-4034457CA70E}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
(tutorial - issue 829): - replaced the pop variable by population everywhere in the tutorial and in examples data. - replaced the s_population variable by demography_session everywhere in the tutorial. - replaced the demo_eurostat variable by demography_eurostat everywhere in the tutorial.
</commit_message>
<xml_diff>
--- a/larray/tests/data/births_and_deaths.xlsx
+++ b/larray/tests/data/births_and_deaths.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ald\Projects\larray\larray\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CF88169-372B-498A-87CF-E26639E34B81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{02C290C4-908F-4A5D-9727-3D9CAE3E3412}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{5CD7B718-4268-44E7-9AF7-549DB247CE6F}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="12675" activeTab="1" xr2:uid="{C85E7F1D-7EF4-469F-934E-2317D9EFA5E4}"/>
   </bookViews>
   <sheets>
     <sheet name="births" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165C2292-4DE4-4BAA-8B67-A256A9BEB0AF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084593C6-F637-4803-992C-67A7198C29CC}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -535,7 +535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{510F0CAE-B993-4579-A875-4034457CA70E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF89640-B556-4155-8AED-FA5591022461}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>